<commit_message>
Ultimos ajustes a la funcionalidad de registrar
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criss\Documents\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEA669B-A4AD-4C3A-8B14-0432645AF794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA12B342-8375-4B28-8BD2-0160E95D0292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,20 +425,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Funcionamiento de el escaneo de codigo
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criss\Documents\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ts3plus\Documents\app-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA12B342-8375-4B28-8BD2-0160E95D0292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1408B2-8669-44E2-9107-A2E3EE4C7CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23610" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ESTADO</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
   <si>
     <t>NOMBRES Y APELLIDOS</t>
@@ -418,7 +421,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -426,7 +429,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -462,6 +465,9 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Añadido de formato a las imagenes
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ts3plus\Documents\app-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criss\Documents\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1408B2-8669-44E2-9107-A2E3EE4C7CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA061C25-02E0-473B-AED9-A3156E7E9EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23610" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE" sheetId="1" r:id="rId1"/>
@@ -427,9 +427,24 @@
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Funcionalidad de registrar usuario completa (Falta que deje descargar los QR)
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -1,87 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criss\Documents\app\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA061C25-02E0-473B-AED9-A3156E7E9EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BASE" sheetId="1" r:id="rId1"/>
+    <sheet name="BASE" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NOMBRES Y APELLIDOS</t>
-  </si>
-  <si>
-    <t>CEDULA</t>
-  </si>
-  <si>
-    <t>EMPRESA</t>
-  </si>
-  <si>
-    <t>TIPO DE TRANSPORTE</t>
-  </si>
-  <si>
-    <t>PLACA</t>
-  </si>
-  <si>
-    <t>TARJETA DE PROPIEDAD</t>
-  </si>
-  <si>
-    <t>CATEGORIA(S)</t>
-  </si>
-  <si>
-    <t>FECHA DE VENCIMIENTO</t>
-  </si>
-  <si>
-    <t>SOAT</t>
-  </si>
-  <si>
-    <t>TECNOMECANICA</t>
-  </si>
-  <si>
-    <t>OBSERVACIONES</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,70 +420,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTADO</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>NOMBRES Y APELLIDOS</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>CEDULA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO DE TRANSPORTE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PLACA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>TARJETA DE PROPIEDAD</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>CATEGORIA(S)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA DE VENCIMIENTO</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SOAT</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>TECNOMECANICA</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OBSERVACIONES</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Cristopher Soto</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1193108338</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>TS3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>SCC15F</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>56456423165</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025/02/27</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025/02/19</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2025/02/20</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Añadido de la funcionalidad Cargue Masivo
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ts3plus\Documents\app-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criss\Documents\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412A1D0A-D2D9-48BC-B8EC-E028636A90DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D6D6A7-C802-4774-841E-7D7CF1B46E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3840" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE" sheetId="1" r:id="rId1"/>
@@ -424,15 +424,12 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Funcionamiento completo de el cargue masivo
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criss\Documents\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D6D6A7-C802-4774-841E-7D7CF1B46E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50578F22-7FB8-4494-8ACF-A468D1EC968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Funcionalidad de Usuarios registrados (Ver QR, Eliminar Usuarios, Ver usuarios creados)
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -1,87 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\criss\Documents\app\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50578F22-7FB8-4494-8ACF-A468D1EC968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BASE" sheetId="1" r:id="rId1"/>
+    <sheet name="BASE" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NOMBRES Y APELLIDOS</t>
-  </si>
-  <si>
-    <t>CEDULA</t>
-  </si>
-  <si>
-    <t>EMPRESA</t>
-  </si>
-  <si>
-    <t>TIPO DE TRANSPORTE</t>
-  </si>
-  <si>
-    <t>PLACA</t>
-  </si>
-  <si>
-    <t>TARJETA DE PROPIEDAD</t>
-  </si>
-  <si>
-    <t>CATEGORIA(S)</t>
-  </si>
-  <si>
-    <t>FECHA DE VENCIMIENTO</t>
-  </si>
-  <si>
-    <t>SOAT</t>
-  </si>
-  <si>
-    <t>TECNOMECANICA</t>
-  </si>
-  <si>
-    <t>OBSERVACIONES</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,55 +420,262 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ESTADO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CEDULA</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>NOMBRES Y APELLIDOS</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO DE TRANSPORTE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PLACA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>TARJETA DE PROPIEDAD</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>CATEGORIA(S)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA DE VENCIMIENTO</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SOAT</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>TECNOMECANICA</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OBSERVACIONES</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>8000000</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1193108338</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Cristopher Soto</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>TS3</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>SCC15F</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>654563456</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2025/02/20</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025/02/19</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2025/02/19</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>8000001</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>213454231</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Juan pablo celeita</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>DFG44H</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>4546</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2025/02/20</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2025/02/19</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2025/02/19</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>8000002</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5456456</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Fernando Soto</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>AAE88U</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>654564</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2025/02/20</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2025/02/19</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025/02/19</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Avance en la funcionalidad de el boton editar
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BASE" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,42 +502,38 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8000000</v>
+        <v>8000007</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Inactivo</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1193108338</t>
-        </is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>77</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Cristopher Soto Viloria</t>
+          <t>rrr</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ts3</t>
+          <t>TS10</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Moto</t>
+          <t>MOTO</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SCC15F</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>73727282</t>
-        </is>
+          <t>SFE44R</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>5465231</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -546,20 +542,248 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025/02/19</t>
+          <t>2025/02/27</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025/02/27</t>
+          <t>2025/03/15</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025/02/04</t>
+          <t>2025/06/13</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>8000008</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>88</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>tytt</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>TS11</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>THV77G</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2025/02/28</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2025/03/16</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2025/06/14</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>8000010</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1111</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>saaa</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>TS13</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>SFE44R</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2025/03/02</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2025/03/18</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025/06/16</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>8000011</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>2222</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>qwewqe</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>TS14</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>THV77G</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2025/03/03</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2025/03/19</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2025/06/17</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>8000013</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4444</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>gjhgjhg</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>TS16</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>SFE44R</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2025/03/05</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2025/03/21</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2025/06/19</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Funcionalidad de editar usuarios añadida
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BASE" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,7 +502,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8000007</v>
+        <v>8000000</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -510,16 +510,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>77</v>
+        <v>1193108338</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>rrr</t>
+          <t>Cristopher Soto Viloria</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>TS10</t>
+          <t>TS3+</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -529,7 +529,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>SFE44R</t>
+          <t>SCC15F</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -542,24 +542,28 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2025/02/27</t>
+          <t>2025/02/20</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025/03/15</t>
+          <t>2025/03/08</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025/06/13</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr"/>
+          <t>2025/06/06</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>ppppp</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8000008</v>
+        <v>8000001</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -567,16 +571,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>tytt</t>
+          <t>pppp</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>TS11</t>
+          <t>TS4</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -586,7 +590,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>THV77G</t>
+          <t>SFE44R</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -599,24 +603,28 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2025/02/28</t>
+          <t>2025/02/21</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025/03/16</t>
+          <t>2025/03/09</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025/06/14</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
+          <t>2025/06/07</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8000010</v>
+        <v>8000002</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -624,16 +632,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1111</v>
+        <v>22</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>saaa</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>TS13</t>
+          <t>TS5</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -643,7 +651,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>SFE44R</t>
+          <t>THV77G</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -656,24 +664,28 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2025/03/02</t>
+          <t>2025/02/22</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025/03/18</t>
+          <t>2025/03/10</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025/06/16</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
+          <t>2025/06/08</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8000011</v>
+        <v>8000003</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -681,16 +693,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2222</v>
+        <v>33</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>qwewqe</t>
+          <t>davis</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>TS14</t>
+          <t>TS6</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -700,7 +712,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>THV77G</t>
+          <t>SCC15F</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -713,24 +725,28 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2025/03/03</t>
+          <t>2025/02/23</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025/03/19</t>
+          <t>2025/03/11</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025/06/17</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
+          <t>2025/06/09</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8000013</v>
+        <v>8000004</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -738,16 +754,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4444</v>
+        <v>44</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>gjhgjhg</t>
+          <t>bbbbbb</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>TS16</t>
+          <t>TS7</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -770,20 +786,634 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
+          <t>2025/02/24</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2025/03/12</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2025/06/10</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>8000005</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>55</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>vvv</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>TS8</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>THV77G</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2025/02/25</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2025/03/13</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2025/06/11</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8000006</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>66</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>bb</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>TS9</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>SCC15F</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2025/02/26</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2025/03/14</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2025/06/12</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8000007</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>77</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>TS10</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>SFE44R</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2025/02/27</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2025/03/15</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2025/06/13</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8000008</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>88</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>tytt</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>TS11</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>THV77G</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2025/02/28</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2025/03/16</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2025/06/14</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>8000009</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>99</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ccc</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>TS12</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>SCC15F</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>2025/03/01</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>2025/03/17</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2025/06/15</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>8000010</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1111</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>saaa</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>TS13</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>SFE44R</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>2025/03/02</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>2025/03/18</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2025/06/16</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>8000011</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>2222</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>qwewqe</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>TS14</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>THV77G</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>2025/03/03</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>2025/03/19</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2025/06/17</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>8000012</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>3333</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>rytrytr</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>TS15</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>SCC15F</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>2025/03/04</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>2025/03/20</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2025/06/18</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>8000013</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>4444</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>gjhgjhg</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>TS16</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>SFE44R</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
           <t>2025/03/05</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>2025/03/21</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>2025/06/19</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>8000014</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Activo</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>55555</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ghkhjk</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>TS17</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>MOTO</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>THV77G</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>5465231</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>2025/03/06</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>2025/03/22</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2025/06/20</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fecha e vencimiento de date a String
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -1,37 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ts3plus\Documents\app-1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F315AC2-F56D-414D-B057-319CF31984ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>CEDULA</t>
+  </si>
+  <si>
+    <t>NOMBRES Y APELLIDOS</t>
+  </si>
+  <si>
+    <t>EMPRESA</t>
+  </si>
+  <si>
+    <t>TIPO DE TRANSPORTE</t>
+  </si>
+  <si>
+    <t>PLACA</t>
+  </si>
+  <si>
+    <t>TARJETA DE PROPIEDAD</t>
+  </si>
+  <si>
+    <t>CATEGORIA(S)</t>
+  </si>
+  <si>
+    <t>FECHA DE VENCIMIENTO</t>
+  </si>
+  <si>
+    <t>SOAT</t>
+  </si>
+  <si>
+    <t>TECNOMECANICA</t>
+  </si>
+  <si>
+    <t>OBSERVACIONES</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +96,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,84 +420,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>ESTADO</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>CEDULA</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>NOMBRES Y APELLIDOS</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>EMPRESA</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>TIPO DE TRANSPORTE</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>PLACA</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>TARJETA DE PROPIEDAD</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>CATEGORIA(S)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>FECHA DE VENCIMIENTO</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>SOAT</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>TECNOMECANICA</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>OBSERVACIONES</t>
-        </is>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se añadio la eliminacion masiva y se corrije errores de cargue masivo y campos vacios
</commit_message>
<xml_diff>
--- a/BASE SOAT.xlsx
+++ b/BASE SOAT.xlsx
@@ -1,87 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ts3plus\Documents\app-1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F315AC2-F56D-414D-B057-319CF31984ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
-    <t>CEDULA</t>
-  </si>
-  <si>
-    <t>NOMBRES Y APELLIDOS</t>
-  </si>
-  <si>
-    <t>EMPRESA</t>
-  </si>
-  <si>
-    <t>TIPO DE TRANSPORTE</t>
-  </si>
-  <si>
-    <t>PLACA</t>
-  </si>
-  <si>
-    <t>TARJETA DE PROPIEDAD</t>
-  </si>
-  <si>
-    <t>CATEGORIA(S)</t>
-  </si>
-  <si>
-    <t>FECHA DE VENCIMIENTO</t>
-  </si>
-  <si>
-    <t>SOAT</t>
-  </si>
-  <si>
-    <t>TECNOMECANICA</t>
-  </si>
-  <si>
-    <t>OBSERVACIONES</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -96,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -420,54 +420,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>ESTADO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CEDULA</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>NOMBRES Y APELLIDOS</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EMPRESA</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>TIPO DE TRANSPORTE</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PLACA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>TARJETA DE PROPIEDAD</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>CATEGORIA(S)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA DE VENCIMIENTO</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>SOAT</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>TECNOMECANICA</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>OBSERVACIONES</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>